<commit_message>
Wijzigingen in zender firmware ivm rfm69w. Voorbereiding zender gemaakt. Libs oké. Todo: mainloop met int check en daarna sleep.
</commit_message>
<xml_diff>
--- a/ISA Ouderen/Zender - Deurbel en Telefoon/Schematic/BOM/ISA Ouderen - Lamp Zender (versie 1).xlsx
+++ b/ISA Ouderen/Zender - Deurbel en Telefoon/Schematic/BOM/ISA Ouderen - Lamp Zender (versie 1).xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="22416"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1720" yWindow="0" windowWidth="25600" windowHeight="16020" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15860" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ISA Ouderen - Lamp Zender.csv" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="96">
   <si>
     <t>Qty</t>
   </si>
@@ -316,7 +316,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;€&quot;\ * #,##0.00_-;_-&quot;€&quot;\ * #,##0.00\-;_-&quot;€&quot;\ * &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -348,8 +348,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -374,6 +381,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8E4BC"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -384,7 +397,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="23">
+  <cellStyleXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -408,8 +421,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -417,8 +432,9 @@
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="23">
+  <cellStyles count="25">
     <cellStyle name="Gevolgde hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -430,6 +446,7 @@
     <cellStyle name="Gevolgde hyperlink" xfId="18" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Gevolgde hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Gevolgde hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -441,6 +458,7 @@
     <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Normaal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -773,7 +791,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -818,20 +836,25 @@
       </c>
     </row>
     <row r="2" spans="1:13">
-      <c r="A2">
+      <c r="A2" s="3">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="7" t="s">
+        <v>89</v>
+      </c>
       <c r="L2" t="s">
         <v>7</v>
       </c>
@@ -942,31 +965,31 @@
       </c>
     </row>
     <row r="6" spans="1:13">
-      <c r="A6" s="5">
+      <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="4">
         <v>0.02</v>
       </c>
-      <c r="G6" s="6">
+      <c r="G6" s="4">
         <f t="shared" si="0"/>
         <v>0.08</v>
       </c>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
-        <v>90</v>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L6" t="s">
         <v>24</v>
@@ -976,31 +999,31 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="5">
+      <c r="A7" s="3">
         <v>2</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="4">
         <v>0.06</v>
       </c>
-      <c r="G7" s="6">
+      <c r="G7" s="4">
         <f t="shared" si="0"/>
         <v>0.12</v>
       </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
-        <v>90</v>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L7" t="s">
         <v>29</v>
@@ -1010,31 +1033,31 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" s="5">
+      <c r="A8" s="3">
         <v>2</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="4">
         <v>0.25</v>
       </c>
-      <c r="G8" s="6">
+      <c r="G8" s="4">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
-        <v>90</v>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L8" t="s">
         <v>34</v>
@@ -1044,31 +1067,31 @@
       </c>
     </row>
     <row r="9" spans="1:13">
-      <c r="A9" s="5">
+      <c r="A9" s="3">
         <v>1</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C9" s="5" t="s">
+      <c r="C9" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="4">
         <v>0.1</v>
       </c>
-      <c r="G9" s="6">
+      <c r="G9" s="4">
         <f t="shared" si="0"/>
         <v>0.1</v>
       </c>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
-        <v>90</v>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L9" t="s">
         <v>39</v>
@@ -1146,31 +1169,31 @@
       </c>
     </row>
     <row r="12" spans="1:13">
-      <c r="A12" s="5">
+      <c r="A12" s="3">
         <v>2</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C12" s="5" t="s">
+      <c r="C12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F12" s="6">
+      <c r="F12" s="4">
         <v>0.76</v>
       </c>
-      <c r="G12" s="6">
+      <c r="G12" s="4">
         <f t="shared" si="0"/>
         <v>1.52</v>
       </c>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5" t="s">
-        <v>90</v>
+      <c r="H12" s="3"/>
+      <c r="I12" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="L12" t="s">
         <v>45</v>
@@ -1248,31 +1271,31 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="5">
+      <c r="A15" s="3">
         <v>2</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C15" s="5" t="s">
+      <c r="C15" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F15" s="6">
+      <c r="F15" s="4">
         <v>1.44</v>
       </c>
-      <c r="G15" s="6">
+      <c r="G15" s="4">
         <f t="shared" si="0"/>
         <v>2.88</v>
       </c>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
-        <v>90</v>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L15" t="s">
         <v>56</v>
@@ -1313,31 +1336,31 @@
       </c>
     </row>
     <row r="17" spans="1:13">
-      <c r="A17" s="5">
+      <c r="A17" s="3">
         <v>1</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F17" s="6">
+      <c r="F17" s="4">
         <v>1.96</v>
       </c>
-      <c r="G17" s="6">
+      <c r="G17" s="4">
         <f t="shared" si="0"/>
         <v>1.96</v>
       </c>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
-        <v>90</v>
+      <c r="H17" s="3"/>
+      <c r="I17" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="L17" t="s">
         <v>64</v>
@@ -1347,31 +1370,31 @@
       </c>
     </row>
     <row r="18" spans="1:13">
-      <c r="A18" s="5">
+      <c r="A18" s="3">
         <v>1</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F18" s="6">
+      <c r="F18" s="4">
         <v>1.96</v>
       </c>
-      <c r="G18" s="6">
+      <c r="G18" s="4">
         <f t="shared" si="0"/>
         <v>1.96</v>
       </c>
-      <c r="H18" s="5"/>
-      <c r="I18" s="5" t="s">
-        <v>90</v>
+      <c r="H18" s="3"/>
+      <c r="I18" s="7" t="s">
+        <v>89</v>
       </c>
       <c r="L18" t="s">
         <v>67</v>
@@ -1412,31 +1435,31 @@
       </c>
     </row>
     <row r="20" spans="1:13">
-      <c r="A20" s="5">
+      <c r="A20" s="3">
         <v>1</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="B20" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C20" s="5" t="s">
+      <c r="C20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F20" s="6">
+      <c r="F20" s="4">
         <v>0.85</v>
       </c>
-      <c r="G20" s="6">
+      <c r="G20" s="4">
         <f t="shared" ref="G20" si="2">F20*A20</f>
         <v>0.85</v>
       </c>
-      <c r="H20" s="5"/>
-      <c r="I20" s="5" t="s">
-        <v>90</v>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L20" t="s">
         <v>72</v>
@@ -1446,31 +1469,31 @@
       </c>
     </row>
     <row r="21" spans="1:13">
-      <c r="A21" s="5">
+      <c r="A21" s="3">
         <v>1</v>
       </c>
-      <c r="B21" s="5" t="s">
+      <c r="B21" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="C21" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="4">
         <v>0.85</v>
       </c>
-      <c r="G21" s="6">
+      <c r="G21" s="4">
         <f t="shared" si="0"/>
         <v>0.85</v>
       </c>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5" t="s">
-        <v>90</v>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L21" t="s">
         <v>72</v>
@@ -1480,31 +1503,31 @@
       </c>
     </row>
     <row r="22" spans="1:13">
-      <c r="A22" s="5">
+      <c r="A22" s="3">
         <v>1</v>
       </c>
-      <c r="B22" s="5" t="s">
+      <c r="B22" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C22" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F22" s="6">
+      <c r="F22" s="4">
         <v>0.25</v>
       </c>
-      <c r="G22" s="6">
+      <c r="G22" s="4">
         <f t="shared" si="0"/>
         <v>0.25</v>
       </c>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5" t="s">
-        <v>90</v>
+      <c r="H22" s="3"/>
+      <c r="I22" s="3" t="s">
+        <v>89</v>
       </c>
       <c r="L22" t="s">
         <v>77</v>

</xml_diff>